<commit_message>
updated files from home
</commit_message>
<xml_diff>
--- a/Seance3-Statistiques_descriptives/Images/Type_association.xlsx
+++ b/Seance3-Statistiques_descriptives/Images/Type_association.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uqam-my.sharepoint.com/personal/adjiwanou_visseho_uqam_ca/Documents/Cours/SOC8655/Automne2022/Seance3_Statistiques descriptives/Images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uqam-my.sharepoint.com/personal/adjiwanou_visseho_uqam_ca/Documents/Cours/SOC8655/Automne2022/Seance3-Statistiques_descriptives/Images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="13_ncr:1_{EAEEE004-1E7B-EE4A-9BF3-E943A6126738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F69D6C7-8F6E-234A-90B5-DCA6C96FC642}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{EAEEE004-1E7B-EE4A-9BF3-E943A6126738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E42452F-2C3C-6B42-B31A-A6B1D27C42AC}"/>
   <bookViews>
-    <workbookView xWindow="16280" yWindow="6420" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{A32BA72A-9ADA-1747-8FD2-9B157721BD3E}"/>
+    <workbookView xWindow="20000" yWindow="7020" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{A32BA72A-9ADA-1747-8FD2-9B157721BD3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -858,7 +858,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -971,7 +971,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="30" t="s">
         <v>46</v>

</xml_diff>